<commit_message>
Accuracy & CM (line 70)
</commit_message>
<xml_diff>
--- a/dataset2.xlsx
+++ b/dataset2.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:G965"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2:A965"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,8 +2657,8 @@
       <c r="F97">
         <v>2.23</v>
       </c>
-      <c r="G97" s="2" t="s">
-        <v>7</v>
+      <c r="G97" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6429,8 +6429,8 @@
       <c r="F261">
         <v>2.2400000000000002</v>
       </c>
-      <c r="G261" s="2" t="s">
-        <v>7</v>
+      <c r="G261" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -11811,8 +11811,8 @@
       <c r="F495">
         <v>2.2599999999999998</v>
       </c>
-      <c r="G495" s="2" t="s">
-        <v>7</v>
+      <c r="G495" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
@@ -22627,7 +22627,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:G965">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>